<commit_message>
diagram body and fixes
</commit_message>
<xml_diff>
--- a/example_data/project_a.xlsx
+++ b/example_data/project_a.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennartschink/Documents/Repositories/Gantt-Maker/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3789E033-E5CA-9041-B134-78C962179FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B93AC84-5EC5-C848-A2DB-632720F63944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2660" windowWidth="27840" windowHeight="16740" xr2:uid="{40A7F958-0BCC-3A49-B27C-EAA23DE19114}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Pitch Product to customer</t>
+  </si>
+  <si>
+    <t>Plan-Start</t>
+  </si>
+  <si>
+    <t>Actual-Start</t>
   </si>
 </sst>
 </file>
@@ -523,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4D157B-9CCD-254B-98DF-BD43ABB0127A}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,11 +540,13 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,14 +556,20 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -568,8 +582,14 @@
       <c r="E2" s="1">
         <v>45505</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1">
+        <v>45505</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -585,8 +605,14 @@
       <c r="E3" s="1">
         <v>45506</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1">
+        <v>45505</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -597,13 +623,19 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>45506</v>
+        <v>45505</v>
       </c>
       <c r="E4" s="1">
         <v>45506</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1">
+        <v>45506</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -614,13 +646,19 @@
         <v>12</v>
       </c>
       <c r="D5" s="1">
+        <v>45510</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45513</v>
+      </c>
+      <c r="F5" s="1">
         <v>45509</v>
       </c>
-      <c r="E5" s="1">
+      <c r="G5" s="1">
         <v>45509</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -631,13 +669,19 @@
         <v>14</v>
       </c>
       <c r="D6" s="1">
+        <v>45506</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45508</v>
+      </c>
+      <c r="F6" s="1">
         <v>45536</v>
       </c>
-      <c r="E6" s="1">
+      <c r="G6" s="1">
         <v>45537</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -648,13 +692,19 @@
         <v>16</v>
       </c>
       <c r="D7" s="1">
+        <v>45509</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45509</v>
+      </c>
+      <c r="F7" s="1">
         <v>45519</v>
       </c>
-      <c r="E7" s="1">
+      <c r="G7" s="1">
         <v>45519</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -665,13 +715,19 @@
         <v>17</v>
       </c>
       <c r="D8" s="1">
+        <v>45509</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45513</v>
+      </c>
+      <c r="F8" s="1">
         <v>45521</v>
       </c>
-      <c r="E8" s="1">
+      <c r="G8" s="1">
         <v>45517</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -682,13 +738,19 @@
         <v>18</v>
       </c>
       <c r="D9" s="1">
+        <v>45518</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45518</v>
+      </c>
+      <c r="F9" s="1">
         <v>45534</v>
       </c>
-      <c r="E9" s="1">
+      <c r="G9" s="1">
         <v>45535</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -704,8 +766,14 @@
       <c r="E10" s="1">
         <v>45537</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1">
+        <v>45536</v>
+      </c>
+      <c r="G10" s="1">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -721,8 +789,14 @@
       <c r="E11" s="1">
         <v>45540</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1">
+        <v>45540</v>
+      </c>
+      <c r="G11" s="1">
+        <v>45540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -733,13 +807,19 @@
         <v>26</v>
       </c>
       <c r="D12" s="1">
+        <v>45541</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45540</v>
+      </c>
+      <c r="F12" s="1">
         <v>45565</v>
       </c>
-      <c r="E12" s="1">
+      <c r="G12" s="1">
         <v>45555</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -750,13 +830,19 @@
         <v>27</v>
       </c>
       <c r="D13" s="1">
+        <v>45541</v>
+      </c>
+      <c r="E13" s="1">
+        <v>45542</v>
+      </c>
+      <c r="F13" s="1">
         <v>45565</v>
       </c>
-      <c r="E13" s="1">
+      <c r="G13" s="1">
         <v>45554</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -767,13 +853,19 @@
         <v>28</v>
       </c>
       <c r="D14" s="1">
+        <v>45541</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45540</v>
+      </c>
+      <c r="F14" s="1">
         <v>45565</v>
       </c>
-      <c r="E14" s="1">
+      <c r="G14" s="1">
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -787,10 +879,16 @@
         <v>45565</v>
       </c>
       <c r="E15" s="1">
+        <v>45560</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45565</v>
+      </c>
+      <c r="G15" s="1">
         <v>45564</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -804,6 +902,12 @@
         <v>45566</v>
       </c>
       <c r="E16" s="1">
+        <v>45566</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45566</v>
+      </c>
+      <c r="G16" s="1">
         <v>45566</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated properties and draw methods, annotaed example file
</commit_message>
<xml_diff>
--- a/example_data/project_a.xlsx
+++ b/example_data/project_a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennartschink/Documents/Repositories/Gantt-Maker/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B93AC84-5EC5-C848-A2DB-632720F63944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A849290-BFDD-8943-BD19-044C5DF675A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2660" windowWidth="27840" windowHeight="16740" xr2:uid="{40A7F958-0BCC-3A49-B27C-EAA23DE19114}"/>
   </bookViews>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4D157B-9CCD-254B-98DF-BD43ABB0127A}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,7 +652,7 @@
         <v>45513</v>
       </c>
       <c r="F5" s="1">
-        <v>45509</v>
+        <v>45511</v>
       </c>
       <c r="G5" s="1">
         <v>45509</v>

</xml_diff>

<commit_message>
added arrows as well as day-numbers in x-axis
</commit_message>
<xml_diff>
--- a/example_data/project_a.xlsx
+++ b/example_data/project_a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennartschink/Documents/Repositories/Gantt-Maker/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A849290-BFDD-8943-BD19-044C5DF675A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC4412C-B403-6A46-A2DA-B5B442FEB6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2660" windowWidth="27840" windowHeight="16740" xr2:uid="{40A7F958-0BCC-3A49-B27C-EAA23DE19114}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>Requirements Engiineering</t>
-  </si>
-  <si>
     <t>2.1</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Actual-Start</t>
+  </si>
+  <si>
+    <t>Requirements Engineering</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,10 +557,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -649,7 +649,7 @@
         <v>45510</v>
       </c>
       <c r="E5" s="1">
-        <v>45513</v>
+        <v>45508</v>
       </c>
       <c r="F5" s="1">
         <v>45511</v>
@@ -666,13 +666,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1">
         <v>45506</v>
       </c>
       <c r="E6" s="1">
-        <v>45508</v>
+        <v>45509</v>
       </c>
       <c r="F6" s="1">
         <v>45536</v>
@@ -683,13 +683,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>45509</v>
@@ -706,13 +706,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1">
         <v>45509</v>
@@ -729,13 +729,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1">
         <v>45518</v>
@@ -752,13 +752,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1">
         <v>45536</v>
@@ -775,13 +775,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1">
         <v>45540</v>
@@ -798,13 +798,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1">
         <v>45541</v>
@@ -821,13 +821,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1">
         <v>45541</v>
@@ -844,13 +844,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1">
         <v>45541</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1">
         <v>45565</v>
@@ -890,13 +890,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D16" s="1">
         <v>45566</v>

</xml_diff>

<commit_message>
editor for gantt diagram. Some improvements.
</commit_message>
<xml_diff>
--- a/example_data/project_a.xlsx
+++ b/example_data/project_a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennartschink/Documents/Repositories/Gantt-Maker/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC4412C-B403-6A46-A2DA-B5B442FEB6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFE5DEC-A644-2441-8C48-37B180E1759F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2660" windowWidth="27840" windowHeight="16740" xr2:uid="{40A7F958-0BCC-3A49-B27C-EAA23DE19114}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A17" sqref="A17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>